<commit_message>
Se agrega scheduler para 5 días
</commit_message>
<xml_diff>
--- a/Medios Ciberseguridad.xlsx
+++ b/Medios Ciberseguridad.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matiasmingo/Desktop/recopilador_ciberseguridad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matiasmingo/Desktop/Banco Central/Analisis_ciberseguridad/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="0" windowWidth="10000" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="14760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fuentes Comunes" sheetId="1" r:id="rId1"/>

</xml_diff>